<commit_message>
DRKAT Update and PRGE psychoeducation plot
</commit_message>
<xml_diff>
--- a/data/drkat_brief_self.xlsx
+++ b/data/drkat_brief_self.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon/BrICC Clinic/BrICC Terms/Spring 2020/pilot_data_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8289A7D9-8DD2-A342-A23E-1E59972FAB46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F887C72-A72A-1F4B-8B0F-0B583934F766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34740" yWindow="5740" windowWidth="27640" windowHeight="15760" xr2:uid="{9988D938-82CA-A942-B621-0AF801FF8327}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -460,6 +460,9 @@
       <c r="B2">
         <v>63</v>
       </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -468,6 +471,9 @@
       <c r="B3">
         <v>60</v>
       </c>
+      <c r="C3">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
@@ -476,6 +482,9 @@
       <c r="B4">
         <v>60</v>
       </c>
+      <c r="C4">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -484,6 +493,9 @@
       <c r="B5">
         <v>50</v>
       </c>
+      <c r="C5">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
@@ -492,6 +504,9 @@
       <c r="B6">
         <v>61</v>
       </c>
+      <c r="C6">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -500,6 +515,9 @@
       <c r="B7">
         <v>60</v>
       </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
@@ -508,6 +526,9 @@
       <c r="B8">
         <v>66</v>
       </c>
+      <c r="C8">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
@@ -516,6 +537,9 @@
       <c r="B9">
         <v>52</v>
       </c>
+      <c r="C9">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
@@ -524,6 +548,9 @@
       <c r="B10">
         <v>59</v>
       </c>
+      <c r="C10">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -532,6 +559,9 @@
       <c r="B11">
         <v>56</v>
       </c>
+      <c r="C11">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
@@ -540,6 +570,9 @@
       <c r="B12">
         <v>59</v>
       </c>
+      <c r="C12">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
@@ -547,6 +580,9 @@
       </c>
       <c r="B13">
         <v>61</v>
+      </c>
+      <c r="C13">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>